<commit_message>
filling out data dict
</commit_message>
<xml_diff>
--- a/lab1/data_dictionary.xlsx
+++ b/lab1/data_dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\az-su\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\az-su\Documents\databased\lab1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="72">
   <si>
     <t>ColName</t>
   </si>
@@ -174,6 +174,72 @@
   </si>
   <si>
     <t xml:space="preserve">genre </t>
+  </si>
+  <si>
+    <t>actors</t>
+  </si>
+  <si>
+    <t>movies</t>
+  </si>
+  <si>
+    <t>keywords</t>
+  </si>
+  <si>
+    <t>keyword</t>
+  </si>
+  <si>
+    <t>fname</t>
+  </si>
+  <si>
+    <t>lname</t>
+  </si>
+  <si>
+    <t>Restriction</t>
+  </si>
+  <si>
+    <t>aka_names</t>
+  </si>
+  <si>
+    <t>series</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>idaka_names</t>
+  </si>
+  <si>
+    <t>moves</t>
+  </si>
+  <si>
+    <t>genres</t>
+  </si>
+  <si>
+    <t>movies_keywords</t>
+  </si>
+  <si>
+    <t>idkeywords</t>
+  </si>
+  <si>
+    <t>idgenres</t>
+  </si>
+  <si>
+    <t>genre</t>
+  </si>
+  <si>
+    <t>aka_titles</t>
+  </si>
+  <si>
+    <t>idaka_titles</t>
+  </si>
+  <si>
+    <t>M-M bridge from character to actor</t>
+  </si>
+  <si>
+    <t>M-M bridge from character to movie</t>
+  </si>
+  <si>
+    <t>M-M bridge from character to series</t>
   </si>
 </sst>
 </file>
@@ -525,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -539,9 +605,10 @@
     <col min="4" max="4" width="12.06640625" customWidth="1"/>
     <col min="5" max="5" width="10.9296875" customWidth="1"/>
     <col min="7" max="7" width="14.19921875" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -564,10 +631,13 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -590,7 +660,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -613,7 +683,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -636,7 +706,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -659,7 +729,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -675,8 +745,11 @@
       <c r="E6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -692,8 +765,11 @@
       <c r="E7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -709,8 +785,14 @@
       <c r="E8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -726,8 +808,14 @@
       <c r="E9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -743,8 +831,14 @@
       <c r="E10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -760,8 +854,14 @@
       <c r="E11" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -777,8 +877,14 @@
       <c r="E12" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -794,8 +900,14 @@
       <c r="E13" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -811,8 +923,14 @@
       <c r="E14" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F14" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -828,8 +946,11 @@
       <c r="E15" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -845,8 +966,11 @@
       <c r="E16" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="I16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -862,8 +986,14 @@
       <c r="E17" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F17" t="s">
+        <v>61</v>
+      </c>
+      <c r="G17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>40</v>
       </c>
@@ -879,8 +1009,14 @@
       <c r="E18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F18" t="s">
+        <v>51</v>
+      </c>
+      <c r="G18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -896,8 +1032,14 @@
       <c r="E19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F19" t="s">
+        <v>51</v>
+      </c>
+      <c r="G19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -913,8 +1055,14 @@
       <c r="E20" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F20" t="s">
+        <v>63</v>
+      </c>
+      <c r="G20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -930,8 +1078,14 @@
       <c r="E21" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F21" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -947,8 +1101,14 @@
       <c r="E22" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F22" t="s">
+        <v>52</v>
+      </c>
+      <c r="G22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -964,8 +1124,14 @@
       <c r="E23" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F23" t="s">
+        <v>52</v>
+      </c>
+      <c r="G23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -981,8 +1147,14 @@
       <c r="E24" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F24" t="s">
+        <v>67</v>
+      </c>
+      <c r="G24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -998,8 +1170,14 @@
       <c r="E25" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F25" t="s">
+        <v>67</v>
+      </c>
+      <c r="G25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -1015,8 +1193,14 @@
       <c r="E26" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F26" t="s">
+        <v>67</v>
+      </c>
+      <c r="G26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>45</v>
       </c>
@@ -1032,8 +1216,14 @@
       <c r="E27" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F27" t="s">
+        <v>67</v>
+      </c>
+      <c r="G27" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -1049,8 +1239,11 @@
       <c r="E28" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="I28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -1066,8 +1259,11 @@
       <c r="E29" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="I29" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -1083,8 +1279,14 @@
       <c r="E30" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F30" t="s">
+        <v>58</v>
+      </c>
+      <c r="G30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>11</v>
       </c>
@@ -1100,8 +1302,14 @@
       <c r="E31" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F31" t="s">
+        <v>58</v>
+      </c>
+      <c r="G31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>47</v>
       </c>
@@ -1117,8 +1325,14 @@
       <c r="E32" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F32" t="s">
+        <v>58</v>
+      </c>
+      <c r="G32" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>48</v>
       </c>
@@ -1134,8 +1348,14 @@
       <c r="E33" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F33" t="s">
+        <v>58</v>
+      </c>
+      <c r="G33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -1151,8 +1371,14 @@
       <c r="E34" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F34" t="s">
+        <v>58</v>
+      </c>
+      <c r="G34" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -1168,8 +1394,14 @@
       <c r="E35" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F35" t="s">
+        <v>62</v>
+      </c>
+      <c r="G35" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>49</v>
       </c>
@@ -1184,6 +1416,12 @@
       </c>
       <c r="E36" t="s">
         <v>17</v>
+      </c>
+      <c r="F36" t="s">
+        <v>62</v>
+      </c>
+      <c r="G36" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>